<commit_message>
updating test example for tutorial example to use converge 2100 methods. added a script to regenerate test file in test_data
</commit_message>
<xml_diff>
--- a/tests/test_data/model.xlsx
+++ b/tests/test_data/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -56,13 +56,16 @@
     <t xml:space="preserve">prefix|Emissions|BC|sector2|suffix</t>
   </si>
   <si>
+    <t xml:space="preserve">prefix|Emissions|BC|suffix</t>
+  </si>
+  <si>
     <t xml:space="preserve">World</t>
   </si>
   <si>
     <t xml:space="preserve">Method</t>
   </si>
   <si>
-    <t xml:space="preserve">reduce_ratio_2080</t>
+    <t xml:space="preserve">reduce_ratio_2100</t>
   </si>
 </sst>
 </file>
@@ -159,21 +162,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="6" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="6" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,46 +335,57 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>10</v>
+        <f aca="false">SUM(F2:F3)</f>
+        <v>21</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>11</v>
+        <f aca="false">SUM(G2:G3)</f>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>12</v>
+        <f aca="false">SUM(H2:H3)</f>
+        <v>25</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>13</v>
+        <f aca="false">SUM(I2:I3)</f>
+        <v>27</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>14</v>
+        <f aca="false">SUM(J2:J3)</f>
+        <v>29</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>15</v>
+        <f aca="false">SUM(K2:K3)</f>
+        <v>31</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>16</v>
+        <f aca="false">SUM(L2:L3)</f>
+        <v>33</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>17</v>
+        <f aca="false">SUM(M2:M3)</f>
+        <v>35</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>18</v>
+        <f aca="false">SUM(N2:N3)</f>
+        <v>37</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>19</v>
+        <f aca="false">SUM(O2:O3)</f>
+        <v>39</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>20</v>
+        <f aca="false">SUM(P2:P3)</f>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,46 +396,157 @@
         <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="H5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="E6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L6" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M6" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N6" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O6" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P6" s="0" t="n">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">SUM(F5:F6)</f>
+        <v>21</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">SUM(G5:G6)</f>
+        <v>23</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">SUM(H5:H6)</f>
+        <v>25</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">SUM(I5:I6)</f>
+        <v>27</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">SUM(J5:J6)</f>
+        <v>29</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">SUM(K5:K6)</f>
+        <v>31</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">SUM(L5:L6)</f>
+        <v>33</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">SUM(M5:M6)</f>
+        <v>35</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false">SUM(N5:N6)</f>
+        <v>37</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">SUM(O5:O6)</f>
+        <v>39</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <f aca="false">SUM(P5:P6)</f>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -444,13 +567,13 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,7 +613,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>